<commit_message>
New PBI Statistics Queries
</commit_message>
<xml_diff>
--- a/SQL/PBI Statistics - Azure/PBI Statistics - Missing Workspace Active Directory Groups.xlsx
+++ b/SQL/PBI Statistics - Azure/PBI Statistics - Missing Workspace Active Directory Groups.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29101"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29108"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kimberlyclark-my.sharepoint.com/personal/steve_wolfe_kcc_com/Documents/Desktop/Code/SQL/PBI Statistics - Azure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="8_{54537649-13BF-4AB8-80CB-CFDA9454A68E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA71EEE5-334A-4527-94F7-120DD704683F}"/>
+  <xr:revisionPtr revIDLastSave="176" documentId="8_{54537649-13BF-4AB8-80CB-CFDA9454A68E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DCA9485-6F02-49F0-8A99-C95EC2800ED6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{C594F4F4-9949-4593-A31F-15D281CFE35F}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="148">
   <si>
     <t>WorkspaceName</t>
   </si>
@@ -127,9 +127,6 @@
     <t>PBI_WS_AP_KOCJ_DM_ADHOC_CONTRIB_P</t>
   </si>
   <si>
-    <t>Mail Sent</t>
-  </si>
-  <si>
     <t>AP KOCJ MAINT - D</t>
   </si>
   <si>
@@ -175,9 +172,6 @@
     <t>PBI_WS_EMEA_KCP_CX_Reporting_ADHOC_VIEWER_P</t>
   </si>
   <si>
-    <t>Mail sent</t>
-  </si>
-  <si>
     <t>GL COMMON CERTIFIED DATASETS - D</t>
   </si>
   <si>
@@ -190,7 +184,7 @@
     <t>PBI_WS_GL_COMMON_CERTIFIED_DATASETS_CONTRIB_N</t>
   </si>
   <si>
-    <t>Requested for AD Groups</t>
+    <t>AD Group is not required</t>
   </si>
   <si>
     <t>GL COMMON CERTIFIED DATASETS - Q</t>
@@ -400,6 +394,9 @@
     <t>PBI_WS_NA_RGM_APP_REPORTING_ADHOC_CONTRIB_P</t>
   </si>
   <si>
+    <t>Waiting for reply Mail</t>
+  </si>
+  <si>
     <t>NA RGM DART REPORTING - Adhoc</t>
   </si>
   <si>
@@ -434,6 +431,9 @@
   </si>
   <si>
     <t>Workspaces</t>
+  </si>
+  <si>
+    <t>AD Group is Not Required</t>
   </si>
   <si>
     <t xml:space="preserve">Waiting for Reply </t>
@@ -532,7 +532,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -555,15 +555,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -666,7 +680,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4933A354-5973-4CE5-8EDC-01C3C337BE2C}" name="Missing_Viewer_or_Contributor" displayName="Missing_Viewer_or_Contributor" ref="A1:I37" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:I37" xr:uid="{4933A354-5973-4CE5-8EDC-01C3C337BE2C}"/>
+  <autoFilter ref="A1:I37" xr:uid="{4933A354-5973-4CE5-8EDC-01C3C337BE2C}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="Deleted"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2A2A993F-CD0B-46BF-878C-97011C797D45}" uniqueName="1" name="WorkspaceName" queryTableFieldId="1" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{E8BB9476-4678-439C-945D-C0B3593BA52F}" uniqueName="2" name="WorkspaceID" queryTableFieldId="2" dataDxfId="14"/>
@@ -1015,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1DA921B-FBFE-44F1-88C4-211554DCA885}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A5" sqref="A5:A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1062,7 +1082,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" hidden="1">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1085,7 +1105,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" hidden="1">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1108,7 +1128,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" hidden="1">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1128,15 +1148,15 @@
         <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
         <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -1145,30 +1165,30 @@
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
         <v>20</v>
       </c>
       <c r="H5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" hidden="1">
+      <c r="A6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
         <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
@@ -1177,21 +1197,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" hidden="1">
       <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
         <v>35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
@@ -1200,92 +1220,92 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" hidden="1">
       <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
         <v>37</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
         <v>38</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
-        <v>39</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
       </c>
       <c r="H8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" hidden="1">
+      <c r="A9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" hidden="1">
+      <c r="A10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" hidden="1">
       <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
         <v>48</v>
-      </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" t="s">
-        <v>50</v>
       </c>
       <c r="G11" t="s">
         <v>20</v>
@@ -1296,203 +1316,203 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G12" t="s">
         <v>20</v>
       </c>
       <c r="H12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G13" t="s">
         <v>20</v>
       </c>
       <c r="H13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" hidden="1">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G14" t="s">
         <v>20</v>
       </c>
       <c r="H14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" hidden="1">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G15" t="s">
         <v>20</v>
       </c>
       <c r="H15" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" t="s">
         <v>62</v>
-      </c>
-      <c r="B16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" t="s">
-        <v>64</v>
       </c>
       <c r="G16" t="s">
         <v>14</v>
       </c>
       <c r="H16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" t="s">
         <v>65</v>
-      </c>
-      <c r="B17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" t="s">
-        <v>67</v>
       </c>
       <c r="G17" t="s">
         <v>14</v>
       </c>
       <c r="H17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" hidden="1">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G18" t="s">
         <v>14</v>
       </c>
       <c r="H18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" hidden="1">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G19" t="s">
         <v>14</v>
       </c>
       <c r="H19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="2" customFormat="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="2" customFormat="1" hidden="1">
       <c r="A20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>14</v>
@@ -1501,395 +1521,405 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" hidden="1">
       <c r="A21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
         <v>76</v>
-      </c>
-      <c r="B21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" t="s">
-        <v>78</v>
       </c>
       <c r="G21" t="s">
         <v>20</v>
       </c>
       <c r="H21" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" t="s">
         <v>79</v>
-      </c>
-      <c r="B22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" t="s">
-        <v>81</v>
       </c>
       <c r="G22" t="s">
         <v>14</v>
       </c>
       <c r="H22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" t="s">
         <v>83</v>
-      </c>
-      <c r="B23" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" t="s">
-        <v>85</v>
       </c>
       <c r="G23" t="s">
         <v>14</v>
       </c>
       <c r="H23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" t="s">
         <v>86</v>
-      </c>
-      <c r="B24" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" t="s">
-        <v>88</v>
       </c>
       <c r="G24" t="s">
         <v>14</v>
       </c>
       <c r="H24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="1" customFormat="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="1" customFormat="1" hidden="1">
       <c r="A25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H25" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G26" t="s">
         <v>14</v>
       </c>
       <c r="H26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G27" t="s">
         <v>14</v>
       </c>
       <c r="H27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" t="s">
         <v>97</v>
-      </c>
-      <c r="B28" t="s">
-        <v>98</v>
-      </c>
-      <c r="C28" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" t="s">
-        <v>99</v>
       </c>
       <c r="G28" t="s">
         <v>14</v>
       </c>
       <c r="H28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" hidden="1">
       <c r="A29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" t="s">
         <v>100</v>
-      </c>
-      <c r="B29" t="s">
-        <v>101</v>
-      </c>
-      <c r="C29" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" t="s">
-        <v>102</v>
       </c>
       <c r="G29" t="s">
         <v>14</v>
       </c>
       <c r="H29" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" t="s">
         <v>103</v>
       </c>
-      <c r="B30" t="s">
+      <c r="D30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" t="s">
         <v>104</v>
-      </c>
-      <c r="C30" t="s">
-        <v>105</v>
-      </c>
-      <c r="D30" t="s">
-        <v>18</v>
-      </c>
-      <c r="E30" t="s">
-        <v>106</v>
       </c>
       <c r="G30" t="s">
         <v>14</v>
       </c>
       <c r="H30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C31" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G31" t="s">
         <v>14</v>
       </c>
       <c r="H31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B32" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C32" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E32" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G32" t="s">
         <v>14</v>
       </c>
       <c r="H32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" hidden="1">
       <c r="A33" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" t="s">
         <v>112</v>
-      </c>
-      <c r="B33" t="s">
-        <v>113</v>
-      </c>
-      <c r="C33" t="s">
-        <v>105</v>
-      </c>
-      <c r="D33" t="s">
-        <v>18</v>
-      </c>
-      <c r="F33" t="s">
-        <v>114</v>
       </c>
       <c r="G33" t="s">
         <v>20</v>
       </c>
       <c r="H33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" hidden="1">
       <c r="A34" t="s">
+        <v>114</v>
+      </c>
+      <c r="B34" t="s">
         <v>115</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
+        <v>103</v>
+      </c>
+      <c r="D34" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" t="s">
         <v>116</v>
-      </c>
-      <c r="C34" t="s">
-        <v>105</v>
-      </c>
-      <c r="D34" t="s">
-        <v>18</v>
-      </c>
-      <c r="F34" t="s">
-        <v>117</v>
       </c>
       <c r="G34" t="s">
         <v>20</v>
       </c>
       <c r="H34" t="s">
-        <v>45</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
+        <v>117</v>
+      </c>
+      <c r="B35" t="s">
         <v>118</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" t="s">
         <v>119</v>
-      </c>
-      <c r="C35" t="s">
-        <v>105</v>
-      </c>
-      <c r="D35" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" t="s">
-        <v>120</v>
       </c>
       <c r="G35" t="s">
         <v>14</v>
       </c>
       <c r="H35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36" t="s">
         <v>121</v>
       </c>
-      <c r="B36" t="s">
-        <v>122</v>
-      </c>
       <c r="C36" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D36" t="s">
         <v>12</v>
       </c>
       <c r="F36" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G36" t="s">
         <v>20</v>
       </c>
       <c r="H36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
+        <v>123</v>
+      </c>
+      <c r="B37" t="s">
         <v>124</v>
       </c>
-      <c r="B37" t="s">
-        <v>125</v>
-      </c>
       <c r="C37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F37" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G37" t="s">
         <v>20</v>
       </c>
       <c r="H37" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="E40" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="E41" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1905,7 +1935,7 @@
   <dimension ref="I11:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1916,7 +1946,7 @@
   <sheetData>
     <row r="11" spans="9:10">
       <c r="I11" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>7</v>
@@ -1924,7 +1954,7 @@
     </row>
     <row r="12" spans="9:10">
       <c r="I12" s="3">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>15</v>
@@ -1935,20 +1965,20 @@
         <v>17</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="9:10">
       <c r="I14" s="3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="9:10">
       <c r="I15" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>127</v>
@@ -2369,10 +2399,10 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
         <v>25</v>
-      </c>
-      <c r="B18" t="s">
-        <v>26</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -2392,10 +2422,10 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
         <v>25</v>
-      </c>
-      <c r="B19" t="s">
-        <v>26</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
@@ -2415,10 +2445,10 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
         <v>25</v>
-      </c>
-      <c r="B20" t="s">
-        <v>26</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
@@ -2438,10 +2468,10 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
         <v>25</v>
-      </c>
-      <c r="B21" t="s">
-        <v>26</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
@@ -2450,7 +2480,7 @@
         <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F21" t="s">
         <v>136</v>
@@ -2461,10 +2491,10 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
         <v>25</v>
-      </c>
-      <c r="B22" t="s">
-        <v>26</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
@@ -2484,16 +2514,16 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
         <v>29</v>
-      </c>
-      <c r="B23" t="s">
-        <v>30</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E23" t="s">
         <v>131</v>
@@ -2507,16 +2537,16 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
         <v>29</v>
-      </c>
-      <c r="B24" t="s">
-        <v>30</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E24" t="s">
         <v>134</v>
@@ -2530,16 +2560,16 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
         <v>29</v>
-      </c>
-      <c r="B25" t="s">
-        <v>30</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E25" t="s">
         <v>135</v>
@@ -2553,19 +2583,19 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
         <v>29</v>
-      </c>
-      <c r="B26" t="s">
-        <v>30</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
       </c>
       <c r="D26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" t="s">
         <v>31</v>
-      </c>
-      <c r="E26" t="s">
-        <v>32</v>
       </c>
       <c r="F26" t="s">
         <v>138</v>
@@ -2576,16 +2606,16 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
         <v>29</v>
-      </c>
-      <c r="B27" t="s">
-        <v>30</v>
       </c>
       <c r="C27" t="s">
         <v>11</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E27" t="s">
         <v>139</v>
@@ -2599,16 +2629,16 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
         <v>33</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>34</v>
       </c>
-      <c r="C28" t="s">
-        <v>35</v>
-      </c>
       <c r="D28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E28" t="s">
         <v>131</v>
@@ -2622,16 +2652,16 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
         <v>33</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>34</v>
       </c>
-      <c r="C29" t="s">
-        <v>35</v>
-      </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E29" t="s">
         <v>134</v>
@@ -2645,16 +2675,16 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
         <v>33</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>34</v>
       </c>
-      <c r="C30" t="s">
-        <v>35</v>
-      </c>
       <c r="D30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E30" t="s">
         <v>135</v>
@@ -2668,19 +2698,19 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
         <v>33</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>34</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" t="s">
         <v>35</v>
-      </c>
-      <c r="D31" t="s">
-        <v>31</v>
-      </c>
-      <c r="E31" t="s">
-        <v>36</v>
       </c>
       <c r="F31" t="s">
         <v>138</v>
@@ -2691,16 +2721,16 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
         <v>33</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>34</v>
       </c>
-      <c r="C32" t="s">
-        <v>35</v>
-      </c>
       <c r="D32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E32" t="s">
         <v>139</v>
@@ -2714,13 +2744,13 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" t="s">
         <v>37</v>
       </c>
-      <c r="B33" t="s">
-        <v>38</v>
-      </c>
       <c r="C33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D33" t="s">
         <v>18</v>
@@ -2737,13 +2767,13 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="B34" t="s">
-        <v>38</v>
-      </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D34" t="s">
         <v>18</v>
@@ -2760,13 +2790,13 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" t="s">
         <v>37</v>
       </c>
-      <c r="B35" t="s">
-        <v>38</v>
-      </c>
       <c r="C35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D35" t="s">
         <v>18</v>
@@ -2783,19 +2813,19 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
         <v>37</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" t="s">
         <v>38</v>
-      </c>
-      <c r="C36" t="s">
-        <v>35</v>
-      </c>
-      <c r="D36" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" t="s">
-        <v>39</v>
       </c>
       <c r="F36" t="s">
         <v>138</v>
@@ -2806,13 +2836,13 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
         <v>37</v>
       </c>
-      <c r="B37" t="s">
-        <v>38</v>
-      </c>
       <c r="C37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D37" t="s">
         <v>18</v>
@@ -2829,13 +2859,13 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" t="s">
         <v>41</v>
-      </c>
-      <c r="B38" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" t="s">
-        <v>43</v>
       </c>
       <c r="D38" t="s">
         <v>12</v>
@@ -2852,13 +2882,13 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" t="s">
         <v>41</v>
-      </c>
-      <c r="B39" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" t="s">
-        <v>43</v>
       </c>
       <c r="D39" t="s">
         <v>12</v>
@@ -2875,13 +2905,13 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" t="s">
         <v>41</v>
-      </c>
-      <c r="B40" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" t="s">
-        <v>43</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
@@ -2898,13 +2928,13 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" t="s">
         <v>41</v>
-      </c>
-      <c r="B41" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" t="s">
-        <v>43</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>
@@ -2921,19 +2951,19 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" t="s">
         <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>42</v>
-      </c>
-      <c r="C42" t="s">
-        <v>43</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
       </c>
       <c r="E42" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F42" t="s">
         <v>136</v>
@@ -2944,13 +2974,13 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" t="s">
         <v>41</v>
-      </c>
-      <c r="B43" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" t="s">
-        <v>43</v>
       </c>
       <c r="D43" t="s">
         <v>12</v>
@@ -2967,13 +2997,13 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" t="s">
         <v>41</v>
-      </c>
-      <c r="B44" t="s">
-        <v>42</v>
-      </c>
-      <c r="C44" t="s">
-        <v>43</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
@@ -2990,16 +3020,16 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C45" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E45" t="s">
         <v>131</v>
@@ -3013,16 +3043,16 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E46" t="s">
         <v>141</v>
@@ -3036,16 +3066,16 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E47" t="s">
         <v>134</v>
@@ -3059,16 +3089,16 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E48" t="s">
         <v>135</v>
@@ -3082,19 +3112,19 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E49" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F49" t="s">
         <v>136</v>
@@ -3105,16 +3135,16 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B50" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E50" t="s">
         <v>142</v>
@@ -3128,16 +3158,16 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B51" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D51" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E51" t="s">
         <v>139</v>
@@ -3151,13 +3181,13 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B52" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C52" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D52" t="s">
         <v>18</v>
@@ -3174,13 +3204,13 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B53" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C53" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D53" t="s">
         <v>18</v>
@@ -3197,13 +3227,13 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B54" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C54" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D54" t="s">
         <v>18</v>
@@ -3220,19 +3250,19 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
+        <v>46</v>
+      </c>
+      <c r="B55" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D55" t="s">
+        <v>18</v>
+      </c>
+      <c r="E55" t="s">
         <v>48</v>
-      </c>
-      <c r="B55" t="s">
-        <v>49</v>
-      </c>
-      <c r="C55" t="s">
-        <v>43</v>
-      </c>
-      <c r="D55" t="s">
-        <v>18</v>
-      </c>
-      <c r="E55" t="s">
-        <v>50</v>
       </c>
       <c r="F55" t="s">
         <v>136</v>
@@ -3243,13 +3273,13 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B56" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C56" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D56" t="s">
         <v>18</v>
@@ -3266,13 +3296,13 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B57" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C57" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D57" t="s">
         <v>18</v>
@@ -3289,13 +3319,13 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B58" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C58" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
@@ -3312,13 +3342,13 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B59" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C59" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D59" t="s">
         <v>12</v>
@@ -3335,13 +3365,13 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B60" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C60" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D60" t="s">
         <v>12</v>
@@ -3358,19 +3388,19 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B61" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C61" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D61" t="s">
         <v>12</v>
       </c>
       <c r="E61" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F61" t="s">
         <v>136</v>
@@ -3381,13 +3411,13 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B62" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C62" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D62" t="s">
         <v>12</v>
@@ -3404,16 +3434,16 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B63" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C63" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D63" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E63" t="s">
         <v>131</v>
@@ -3427,16 +3457,16 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B64" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C64" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D64" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E64" t="s">
         <v>134</v>
@@ -3450,16 +3480,16 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B65" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C65" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E65" t="s">
         <v>135</v>
@@ -3473,19 +3503,19 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B66" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C66" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D66" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E66" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F66" t="s">
         <v>136</v>
@@ -3496,16 +3526,16 @@
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B67" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C67" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D67" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E67" t="s">
         <v>139</v>
@@ -3519,13 +3549,13 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B68" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C68" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D68" t="s">
         <v>12</v>
@@ -3542,13 +3572,13 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B69" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C69" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D69" t="s">
         <v>12</v>
@@ -3565,13 +3595,13 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B70" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C70" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D70" t="s">
         <v>12</v>
@@ -3588,19 +3618,19 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B71" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C71" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D71" t="s">
         <v>12</v>
       </c>
       <c r="E71" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F71" t="s">
         <v>136</v>
@@ -3611,13 +3641,13 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B72" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C72" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D72" t="s">
         <v>12</v>
@@ -3634,16 +3664,16 @@
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B73" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C73" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D73" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E73" t="s">
         <v>131</v>
@@ -3657,16 +3687,16 @@
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B74" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C74" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D74" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E74" t="s">
         <v>134</v>
@@ -3680,16 +3710,16 @@
     </row>
     <row r="75" spans="1:7">
       <c r="A75" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B75" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C75" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D75" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E75" t="s">
         <v>135</v>
@@ -3703,19 +3733,19 @@
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B76" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C76" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D76" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E76" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F76" t="s">
         <v>136</v>
@@ -3726,16 +3756,16 @@
     </row>
     <row r="77" spans="1:7">
       <c r="A77" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B77" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C77" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D77" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E77" t="s">
         <v>139</v>
@@ -3749,13 +3779,13 @@
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B78" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C78" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D78" t="s">
         <v>18</v>
@@ -3772,13 +3802,13 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B79" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C79" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D79" t="s">
         <v>18</v>
@@ -3795,13 +3825,13 @@
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B80" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C80" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D80" t="s">
         <v>18</v>
@@ -3818,19 +3848,19 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
+        <v>60</v>
+      </c>
+      <c r="B81" t="s">
+        <v>61</v>
+      </c>
+      <c r="C81" t="s">
+        <v>51</v>
+      </c>
+      <c r="D81" t="s">
+        <v>18</v>
+      </c>
+      <c r="E81" t="s">
         <v>62</v>
-      </c>
-      <c r="B81" t="s">
-        <v>63</v>
-      </c>
-      <c r="C81" t="s">
-        <v>53</v>
-      </c>
-      <c r="D81" t="s">
-        <v>18</v>
-      </c>
-      <c r="E81" t="s">
-        <v>64</v>
       </c>
       <c r="F81" t="s">
         <v>138</v>
@@ -3841,13 +3871,13 @@
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B82" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C82" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D82" t="s">
         <v>18</v>
@@ -3864,13 +3894,13 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B83" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C83" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D83" t="s">
         <v>18</v>
@@ -3887,13 +3917,13 @@
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B84" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C84" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D84" t="s">
         <v>18</v>
@@ -3910,13 +3940,13 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B85" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C85" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D85" t="s">
         <v>18</v>
@@ -3933,19 +3963,19 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
+        <v>63</v>
+      </c>
+      <c r="B86" t="s">
+        <v>64</v>
+      </c>
+      <c r="C86" t="s">
+        <v>51</v>
+      </c>
+      <c r="D86" t="s">
+        <v>18</v>
+      </c>
+      <c r="E86" t="s">
         <v>65</v>
-      </c>
-      <c r="B86" t="s">
-        <v>66</v>
-      </c>
-      <c r="C86" t="s">
-        <v>53</v>
-      </c>
-      <c r="D86" t="s">
-        <v>18</v>
-      </c>
-      <c r="E86" t="s">
-        <v>67</v>
       </c>
       <c r="F86" t="s">
         <v>138</v>
@@ -3956,13 +3986,13 @@
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B87" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C87" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D87" t="s">
         <v>18</v>
@@ -3979,13 +4009,13 @@
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B88" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C88" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D88" t="s">
         <v>12</v>
@@ -4002,13 +4032,13 @@
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B89" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C89" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D89" t="s">
         <v>12</v>
@@ -4025,13 +4055,13 @@
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B90" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C90" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D90" t="s">
         <v>12</v>
@@ -4048,19 +4078,19 @@
     </row>
     <row r="91" spans="1:7">
       <c r="A91" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B91" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C91" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D91" t="s">
         <v>12</v>
       </c>
       <c r="E91" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F91" t="s">
         <v>138</v>
@@ -4071,13 +4101,13 @@
     </row>
     <row r="92" spans="1:7">
       <c r="A92" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B92" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C92" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D92" t="s">
         <v>12</v>
@@ -4094,16 +4124,16 @@
     </row>
     <row r="93" spans="1:7">
       <c r="A93" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B93" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C93" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D93" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E93" t="s">
         <v>131</v>
@@ -4117,16 +4147,16 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B94" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C94" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D94" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E94" t="s">
         <v>134</v>
@@ -4140,16 +4170,16 @@
     </row>
     <row r="95" spans="1:7">
       <c r="A95" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B95" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C95" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D95" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E95" t="s">
         <v>135</v>
@@ -4163,19 +4193,19 @@
     </row>
     <row r="96" spans="1:7">
       <c r="A96" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B96" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C96" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D96" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E96" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F96" t="s">
         <v>138</v>
@@ -4186,16 +4216,16 @@
     </row>
     <row r="97" spans="1:7">
       <c r="A97" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B97" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C97" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D97" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E97" t="s">
         <v>139</v>
@@ -4209,13 +4239,13 @@
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B98" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C98" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D98" t="s">
         <v>18</v>
@@ -4232,13 +4262,13 @@
     </row>
     <row r="99" spans="1:7">
       <c r="A99" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B99" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C99" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D99" t="s">
         <v>18</v>
@@ -4255,13 +4285,13 @@
     </row>
     <row r="100" spans="1:7">
       <c r="A100" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B100" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C100" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D100" t="s">
         <v>18</v>
@@ -4278,19 +4308,19 @@
     </row>
     <row r="101" spans="1:7">
       <c r="A101" t="s">
+        <v>71</v>
+      </c>
+      <c r="B101" t="s">
+        <v>72</v>
+      </c>
+      <c r="C101" t="s">
+        <v>51</v>
+      </c>
+      <c r="D101" t="s">
+        <v>18</v>
+      </c>
+      <c r="E101" t="s">
         <v>73</v>
-      </c>
-      <c r="B101" t="s">
-        <v>74</v>
-      </c>
-      <c r="C101" t="s">
-        <v>53</v>
-      </c>
-      <c r="D101" t="s">
-        <v>18</v>
-      </c>
-      <c r="E101" t="s">
-        <v>75</v>
       </c>
       <c r="F101" t="s">
         <v>138</v>
@@ -4301,13 +4331,13 @@
     </row>
     <row r="102" spans="1:7">
       <c r="A102" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B102" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C102" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D102" t="s">
         <v>18</v>
@@ -4324,13 +4354,13 @@
     </row>
     <row r="103" spans="1:7">
       <c r="A103" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B103" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C103" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D103" t="s">
         <v>18</v>
@@ -4347,13 +4377,13 @@
     </row>
     <row r="104" spans="1:7">
       <c r="A104" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B104" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C104" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D104" t="s">
         <v>18</v>
@@ -4370,13 +4400,13 @@
     </row>
     <row r="105" spans="1:7">
       <c r="A105" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B105" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C105" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D105" t="s">
         <v>18</v>
@@ -4393,19 +4423,19 @@
     </row>
     <row r="106" spans="1:7">
       <c r="A106" t="s">
+        <v>74</v>
+      </c>
+      <c r="B106" t="s">
+        <v>75</v>
+      </c>
+      <c r="C106" t="s">
+        <v>51</v>
+      </c>
+      <c r="D106" t="s">
+        <v>18</v>
+      </c>
+      <c r="E106" t="s">
         <v>76</v>
-      </c>
-      <c r="B106" t="s">
-        <v>77</v>
-      </c>
-      <c r="C106" t="s">
-        <v>53</v>
-      </c>
-      <c r="D106" t="s">
-        <v>18</v>
-      </c>
-      <c r="E106" t="s">
-        <v>78</v>
       </c>
       <c r="F106" t="s">
         <v>136</v>
@@ -4416,13 +4446,13 @@
     </row>
     <row r="107" spans="1:7">
       <c r="A107" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B107" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C107" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D107" t="s">
         <v>18</v>
@@ -4439,13 +4469,13 @@
     </row>
     <row r="108" spans="1:7">
       <c r="A108" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B108" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C108" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D108" t="s">
         <v>18</v>
@@ -4462,13 +4492,13 @@
     </row>
     <row r="109" spans="1:7">
       <c r="A109" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B109" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C109" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D109" t="s">
         <v>18</v>
@@ -4485,13 +4515,13 @@
     </row>
     <row r="110" spans="1:7">
       <c r="A110" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B110" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C110" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D110" t="s">
         <v>18</v>
@@ -4508,19 +4538,19 @@
     </row>
     <row r="111" spans="1:7">
       <c r="A111" t="s">
+        <v>77</v>
+      </c>
+      <c r="B111" t="s">
+        <v>78</v>
+      </c>
+      <c r="C111" t="s">
+        <v>51</v>
+      </c>
+      <c r="D111" t="s">
+        <v>18</v>
+      </c>
+      <c r="E111" t="s">
         <v>79</v>
-      </c>
-      <c r="B111" t="s">
-        <v>80</v>
-      </c>
-      <c r="C111" t="s">
-        <v>53</v>
-      </c>
-      <c r="D111" t="s">
-        <v>18</v>
-      </c>
-      <c r="E111" t="s">
-        <v>81</v>
       </c>
       <c r="F111" t="s">
         <v>138</v>
@@ -4531,13 +4561,13 @@
     </row>
     <row r="112" spans="1:7">
       <c r="A112" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B112" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C112" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D112" t="s">
         <v>18</v>
@@ -4554,13 +4584,13 @@
     </row>
     <row r="113" spans="1:7">
       <c r="A113" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B113" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C113" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D113" t="s">
         <v>18</v>
@@ -4577,13 +4607,13 @@
     </row>
     <row r="114" spans="1:7">
       <c r="A114" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B114" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C114" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D114" t="s">
         <v>18</v>
@@ -4600,13 +4630,13 @@
     </row>
     <row r="115" spans="1:7">
       <c r="A115" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B115" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C115" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D115" t="s">
         <v>18</v>
@@ -4623,19 +4653,19 @@
     </row>
     <row r="116" spans="1:7">
       <c r="A116" t="s">
+        <v>81</v>
+      </c>
+      <c r="B116" t="s">
+        <v>82</v>
+      </c>
+      <c r="C116" t="s">
+        <v>51</v>
+      </c>
+      <c r="D116" t="s">
+        <v>18</v>
+      </c>
+      <c r="E116" t="s">
         <v>83</v>
-      </c>
-      <c r="B116" t="s">
-        <v>84</v>
-      </c>
-      <c r="C116" t="s">
-        <v>53</v>
-      </c>
-      <c r="D116" t="s">
-        <v>18</v>
-      </c>
-      <c r="E116" t="s">
-        <v>85</v>
       </c>
       <c r="F116" t="s">
         <v>138</v>
@@ -4646,13 +4676,13 @@
     </row>
     <row r="117" spans="1:7">
       <c r="A117" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B117" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C117" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D117" t="s">
         <v>18</v>
@@ -4669,13 +4699,13 @@
     </row>
     <row r="118" spans="1:7">
       <c r="A118" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B118" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C118" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D118" t="s">
         <v>18</v>
@@ -4692,13 +4722,13 @@
     </row>
     <row r="119" spans="1:7">
       <c r="A119" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B119" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C119" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D119" t="s">
         <v>18</v>
@@ -4715,13 +4745,13 @@
     </row>
     <row r="120" spans="1:7">
       <c r="A120" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B120" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C120" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D120" t="s">
         <v>18</v>
@@ -4738,19 +4768,19 @@
     </row>
     <row r="121" spans="1:7">
       <c r="A121" t="s">
+        <v>84</v>
+      </c>
+      <c r="B121" t="s">
+        <v>85</v>
+      </c>
+      <c r="C121" t="s">
+        <v>51</v>
+      </c>
+      <c r="D121" t="s">
+        <v>18</v>
+      </c>
+      <c r="E121" t="s">
         <v>86</v>
-      </c>
-      <c r="B121" t="s">
-        <v>87</v>
-      </c>
-      <c r="C121" t="s">
-        <v>53</v>
-      </c>
-      <c r="D121" t="s">
-        <v>18</v>
-      </c>
-      <c r="E121" t="s">
-        <v>88</v>
       </c>
       <c r="F121" t="s">
         <v>138</v>
@@ -4761,13 +4791,13 @@
     </row>
     <row r="122" spans="1:7">
       <c r="A122" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B122" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C122" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D122" t="s">
         <v>18</v>
@@ -4784,16 +4814,16 @@
     </row>
     <row r="123" spans="1:7">
       <c r="A123" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B123" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C123" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D123" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E123" t="s">
         <v>131</v>
@@ -4807,16 +4837,16 @@
     </row>
     <row r="124" spans="1:7">
       <c r="A124" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B124" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C124" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D124" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E124" t="s">
         <v>134</v>
@@ -4830,16 +4860,16 @@
     </row>
     <row r="125" spans="1:7">
       <c r="A125" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B125" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C125" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D125" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E125" t="s">
         <v>135</v>
@@ -4853,16 +4883,16 @@
     </row>
     <row r="126" spans="1:7">
       <c r="A126" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B126" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C126" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D126" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E126" t="s">
         <v>144</v>
@@ -4876,19 +4906,19 @@
     </row>
     <row r="127" spans="1:7">
       <c r="A127" t="s">
+        <v>87</v>
+      </c>
+      <c r="B127" t="s">
+        <v>88</v>
+      </c>
+      <c r="C127" t="s">
+        <v>51</v>
+      </c>
+      <c r="D127" t="s">
+        <v>30</v>
+      </c>
+      <c r="E127" t="s">
         <v>89</v>
-      </c>
-      <c r="B127" t="s">
-        <v>90</v>
-      </c>
-      <c r="C127" t="s">
-        <v>53</v>
-      </c>
-      <c r="D127" t="s">
-        <v>31</v>
-      </c>
-      <c r="E127" t="s">
-        <v>91</v>
       </c>
       <c r="F127" t="s">
         <v>136</v>
@@ -4899,13 +4929,13 @@
     </row>
     <row r="128" spans="1:7">
       <c r="A128" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B128" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C128" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D128" t="s">
         <v>12</v>
@@ -4922,13 +4952,13 @@
     </row>
     <row r="129" spans="1:7">
       <c r="A129" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B129" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C129" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D129" t="s">
         <v>12</v>
@@ -4945,13 +4975,13 @@
     </row>
     <row r="130" spans="1:7">
       <c r="A130" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B130" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C130" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D130" t="s">
         <v>12</v>
@@ -4968,19 +4998,19 @@
     </row>
     <row r="131" spans="1:7">
       <c r="A131" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B131" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C131" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D131" t="s">
         <v>12</v>
       </c>
       <c r="E131" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F131" t="s">
         <v>138</v>
@@ -4991,13 +5021,13 @@
     </row>
     <row r="132" spans="1:7">
       <c r="A132" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B132" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C132" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D132" t="s">
         <v>12</v>
@@ -5014,16 +5044,16 @@
     </row>
     <row r="133" spans="1:7">
       <c r="A133" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B133" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C133" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D133" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E133" t="s">
         <v>131</v>
@@ -5037,16 +5067,16 @@
     </row>
     <row r="134" spans="1:7">
       <c r="A134" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B134" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C134" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D134" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E134" t="s">
         <v>134</v>
@@ -5060,16 +5090,16 @@
     </row>
     <row r="135" spans="1:7">
       <c r="A135" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B135" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C135" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D135" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E135" t="s">
         <v>135</v>
@@ -5083,19 +5113,19 @@
     </row>
     <row r="136" spans="1:7">
       <c r="A136" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B136" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C136" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D136" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E136" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F136" t="s">
         <v>138</v>
@@ -5106,16 +5136,16 @@
     </row>
     <row r="137" spans="1:7">
       <c r="A137" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B137" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C137" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D137" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E137" t="s">
         <v>139</v>
@@ -5129,13 +5159,13 @@
     </row>
     <row r="138" spans="1:7">
       <c r="A138" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B138" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C138" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D138" t="s">
         <v>18</v>
@@ -5152,13 +5182,13 @@
     </row>
     <row r="139" spans="1:7">
       <c r="A139" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B139" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C139" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D139" t="s">
         <v>18</v>
@@ -5175,13 +5205,13 @@
     </row>
     <row r="140" spans="1:7">
       <c r="A140" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B140" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C140" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D140" t="s">
         <v>18</v>
@@ -5198,19 +5228,19 @@
     </row>
     <row r="141" spans="1:7">
       <c r="A141" t="s">
+        <v>95</v>
+      </c>
+      <c r="B141" t="s">
+        <v>96</v>
+      </c>
+      <c r="C141" t="s">
+        <v>51</v>
+      </c>
+      <c r="D141" t="s">
+        <v>18</v>
+      </c>
+      <c r="E141" t="s">
         <v>97</v>
-      </c>
-      <c r="B141" t="s">
-        <v>98</v>
-      </c>
-      <c r="C141" t="s">
-        <v>53</v>
-      </c>
-      <c r="D141" t="s">
-        <v>18</v>
-      </c>
-      <c r="E141" t="s">
-        <v>99</v>
       </c>
       <c r="F141" t="s">
         <v>138</v>
@@ -5221,13 +5251,13 @@
     </row>
     <row r="142" spans="1:7">
       <c r="A142" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B142" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C142" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D142" t="s">
         <v>18</v>
@@ -5244,13 +5274,13 @@
     </row>
     <row r="143" spans="1:7">
       <c r="A143" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B143" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C143" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D143" t="s">
         <v>18</v>
@@ -5267,13 +5297,13 @@
     </row>
     <row r="144" spans="1:7">
       <c r="A144" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B144" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C144" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D144" t="s">
         <v>18</v>
@@ -5290,13 +5320,13 @@
     </row>
     <row r="145" spans="1:7">
       <c r="A145" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B145" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C145" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D145" t="s">
         <v>18</v>
@@ -5313,19 +5343,19 @@
     </row>
     <row r="146" spans="1:7">
       <c r="A146" t="s">
+        <v>98</v>
+      </c>
+      <c r="B146" t="s">
+        <v>99</v>
+      </c>
+      <c r="C146" t="s">
+        <v>51</v>
+      </c>
+      <c r="D146" t="s">
+        <v>18</v>
+      </c>
+      <c r="E146" t="s">
         <v>100</v>
-      </c>
-      <c r="B146" t="s">
-        <v>101</v>
-      </c>
-      <c r="C146" t="s">
-        <v>53</v>
-      </c>
-      <c r="D146" t="s">
-        <v>18</v>
-      </c>
-      <c r="E146" t="s">
-        <v>102</v>
       </c>
       <c r="F146" t="s">
         <v>138</v>
@@ -5336,13 +5366,13 @@
     </row>
     <row r="147" spans="1:7">
       <c r="A147" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B147" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C147" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D147" t="s">
         <v>18</v>
@@ -5359,13 +5389,13 @@
     </row>
     <row r="148" spans="1:7">
       <c r="A148" t="s">
+        <v>101</v>
+      </c>
+      <c r="B148" t="s">
+        <v>102</v>
+      </c>
+      <c r="C148" t="s">
         <v>103</v>
-      </c>
-      <c r="B148" t="s">
-        <v>104</v>
-      </c>
-      <c r="C148" t="s">
-        <v>105</v>
       </c>
       <c r="D148" t="s">
         <v>18</v>
@@ -5382,13 +5412,13 @@
     </row>
     <row r="149" spans="1:7">
       <c r="A149" t="s">
+        <v>101</v>
+      </c>
+      <c r="B149" t="s">
+        <v>102</v>
+      </c>
+      <c r="C149" t="s">
         <v>103</v>
-      </c>
-      <c r="B149" t="s">
-        <v>104</v>
-      </c>
-      <c r="C149" t="s">
-        <v>105</v>
       </c>
       <c r="D149" t="s">
         <v>18</v>
@@ -5405,13 +5435,13 @@
     </row>
     <row r="150" spans="1:7">
       <c r="A150" t="s">
+        <v>101</v>
+      </c>
+      <c r="B150" t="s">
+        <v>102</v>
+      </c>
+      <c r="C150" t="s">
         <v>103</v>
-      </c>
-      <c r="B150" t="s">
-        <v>104</v>
-      </c>
-      <c r="C150" t="s">
-        <v>105</v>
       </c>
       <c r="D150" t="s">
         <v>18</v>
@@ -5428,19 +5458,19 @@
     </row>
     <row r="151" spans="1:7">
       <c r="A151" t="s">
+        <v>101</v>
+      </c>
+      <c r="B151" t="s">
+        <v>102</v>
+      </c>
+      <c r="C151" t="s">
         <v>103</v>
       </c>
-      <c r="B151" t="s">
+      <c r="D151" t="s">
+        <v>18</v>
+      </c>
+      <c r="E151" t="s">
         <v>104</v>
-      </c>
-      <c r="C151" t="s">
-        <v>105</v>
-      </c>
-      <c r="D151" t="s">
-        <v>18</v>
-      </c>
-      <c r="E151" t="s">
-        <v>106</v>
       </c>
       <c r="F151" t="s">
         <v>138</v>
@@ -5451,13 +5481,13 @@
     </row>
     <row r="152" spans="1:7">
       <c r="A152" t="s">
+        <v>101</v>
+      </c>
+      <c r="B152" t="s">
+        <v>102</v>
+      </c>
+      <c r="C152" t="s">
         <v>103</v>
-      </c>
-      <c r="B152" t="s">
-        <v>104</v>
-      </c>
-      <c r="C152" t="s">
-        <v>105</v>
       </c>
       <c r="D152" t="s">
         <v>18</v>
@@ -5474,13 +5504,13 @@
     </row>
     <row r="153" spans="1:7">
       <c r="A153" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B153" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C153" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D153" t="s">
         <v>12</v>
@@ -5497,13 +5527,13 @@
     </row>
     <row r="154" spans="1:7">
       <c r="A154" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B154" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C154" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D154" t="s">
         <v>12</v>
@@ -5520,13 +5550,13 @@
     </row>
     <row r="155" spans="1:7">
       <c r="A155" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B155" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C155" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D155" t="s">
         <v>12</v>
@@ -5543,19 +5573,19 @@
     </row>
     <row r="156" spans="1:7">
       <c r="A156" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B156" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C156" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D156" t="s">
         <v>12</v>
       </c>
       <c r="E156" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F156" t="s">
         <v>138</v>
@@ -5566,13 +5596,13 @@
     </row>
     <row r="157" spans="1:7">
       <c r="A157" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B157" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C157" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D157" t="s">
         <v>12</v>
@@ -5589,16 +5619,16 @@
     </row>
     <row r="158" spans="1:7">
       <c r="A158" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B158" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C158" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D158" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E158" t="s">
         <v>131</v>
@@ -5612,16 +5642,16 @@
     </row>
     <row r="159" spans="1:7">
       <c r="A159" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B159" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C159" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D159" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E159" t="s">
         <v>134</v>
@@ -5635,16 +5665,16 @@
     </row>
     <row r="160" spans="1:7">
       <c r="A160" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B160" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C160" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D160" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E160" t="s">
         <v>135</v>
@@ -5658,19 +5688,19 @@
     </row>
     <row r="161" spans="1:7">
       <c r="A161" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B161" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C161" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D161" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E161" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F161" t="s">
         <v>138</v>
@@ -5681,16 +5711,16 @@
     </row>
     <row r="162" spans="1:7">
       <c r="A162" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B162" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C162" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D162" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E162" t="s">
         <v>139</v>
@@ -5704,13 +5734,13 @@
     </row>
     <row r="163" spans="1:7">
       <c r="A163" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B163" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C163" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D163" t="s">
         <v>18</v>
@@ -5727,13 +5757,13 @@
     </row>
     <row r="164" spans="1:7">
       <c r="A164" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B164" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C164" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D164" t="s">
         <v>18</v>
@@ -5750,13 +5780,13 @@
     </row>
     <row r="165" spans="1:7">
       <c r="A165" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B165" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C165" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D165" t="s">
         <v>18</v>
@@ -5773,13 +5803,13 @@
     </row>
     <row r="166" spans="1:7">
       <c r="A166" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B166" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C166" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D166" t="s">
         <v>18</v>
@@ -5796,19 +5826,19 @@
     </row>
     <row r="167" spans="1:7">
       <c r="A167" t="s">
+        <v>110</v>
+      </c>
+      <c r="B167" t="s">
+        <v>111</v>
+      </c>
+      <c r="C167" t="s">
+        <v>103</v>
+      </c>
+      <c r="D167" t="s">
+        <v>18</v>
+      </c>
+      <c r="E167" t="s">
         <v>112</v>
-      </c>
-      <c r="B167" t="s">
-        <v>113</v>
-      </c>
-      <c r="C167" t="s">
-        <v>105</v>
-      </c>
-      <c r="D167" t="s">
-        <v>18</v>
-      </c>
-      <c r="E167" t="s">
-        <v>114</v>
       </c>
       <c r="F167" t="s">
         <v>136</v>
@@ -5819,13 +5849,13 @@
     </row>
     <row r="168" spans="1:7">
       <c r="A168" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B168" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C168" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D168" t="s">
         <v>18</v>
@@ -5842,13 +5872,13 @@
     </row>
     <row r="169" spans="1:7">
       <c r="A169" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B169" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C169" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D169" t="s">
         <v>18</v>
@@ -5865,13 +5895,13 @@
     </row>
     <row r="170" spans="1:7">
       <c r="A170" t="s">
+        <v>114</v>
+      </c>
+      <c r="B170" t="s">
         <v>115</v>
       </c>
-      <c r="B170" t="s">
-        <v>116</v>
-      </c>
       <c r="C170" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D170" t="s">
         <v>18</v>
@@ -5888,13 +5918,13 @@
     </row>
     <row r="171" spans="1:7">
       <c r="A171" t="s">
+        <v>114</v>
+      </c>
+      <c r="B171" t="s">
         <v>115</v>
       </c>
-      <c r="B171" t="s">
-        <v>116</v>
-      </c>
       <c r="C171" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D171" t="s">
         <v>18</v>
@@ -5911,13 +5941,13 @@
     </row>
     <row r="172" spans="1:7">
       <c r="A172" t="s">
+        <v>114</v>
+      </c>
+      <c r="B172" t="s">
         <v>115</v>
       </c>
-      <c r="B172" t="s">
-        <v>116</v>
-      </c>
       <c r="C172" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D172" t="s">
         <v>18</v>
@@ -5934,19 +5964,19 @@
     </row>
     <row r="173" spans="1:7">
       <c r="A173" t="s">
+        <v>114</v>
+      </c>
+      <c r="B173" t="s">
         <v>115</v>
       </c>
-      <c r="B173" t="s">
+      <c r="C173" t="s">
+        <v>103</v>
+      </c>
+      <c r="D173" t="s">
+        <v>18</v>
+      </c>
+      <c r="E173" t="s">
         <v>116</v>
-      </c>
-      <c r="C173" t="s">
-        <v>105</v>
-      </c>
-      <c r="D173" t="s">
-        <v>18</v>
-      </c>
-      <c r="E173" t="s">
-        <v>117</v>
       </c>
       <c r="F173" t="s">
         <v>136</v>
@@ -5957,13 +5987,13 @@
     </row>
     <row r="174" spans="1:7">
       <c r="A174" t="s">
+        <v>114</v>
+      </c>
+      <c r="B174" t="s">
         <v>115</v>
       </c>
-      <c r="B174" t="s">
-        <v>116</v>
-      </c>
       <c r="C174" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D174" t="s">
         <v>18</v>
@@ -5980,13 +6010,13 @@
     </row>
     <row r="175" spans="1:7">
       <c r="A175" t="s">
+        <v>117</v>
+      </c>
+      <c r="B175" t="s">
         <v>118</v>
       </c>
-      <c r="B175" t="s">
-        <v>119</v>
-      </c>
       <c r="C175" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D175" t="s">
         <v>18</v>
@@ -6003,13 +6033,13 @@
     </row>
     <row r="176" spans="1:7">
       <c r="A176" t="s">
+        <v>117</v>
+      </c>
+      <c r="B176" t="s">
         <v>118</v>
       </c>
-      <c r="B176" t="s">
-        <v>119</v>
-      </c>
       <c r="C176" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D176" t="s">
         <v>18</v>
@@ -6026,13 +6056,13 @@
     </row>
     <row r="177" spans="1:7">
       <c r="A177" t="s">
+        <v>117</v>
+      </c>
+      <c r="B177" t="s">
         <v>118</v>
       </c>
-      <c r="B177" t="s">
-        <v>119</v>
-      </c>
       <c r="C177" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D177" t="s">
         <v>18</v>
@@ -6049,19 +6079,19 @@
     </row>
     <row r="178" spans="1:7">
       <c r="A178" t="s">
+        <v>117</v>
+      </c>
+      <c r="B178" t="s">
         <v>118</v>
       </c>
-      <c r="B178" t="s">
+      <c r="C178" t="s">
+        <v>103</v>
+      </c>
+      <c r="D178" t="s">
+        <v>18</v>
+      </c>
+      <c r="E178" t="s">
         <v>119</v>
-      </c>
-      <c r="C178" t="s">
-        <v>105</v>
-      </c>
-      <c r="D178" t="s">
-        <v>18</v>
-      </c>
-      <c r="E178" t="s">
-        <v>120</v>
       </c>
       <c r="F178" t="s">
         <v>138</v>
@@ -6072,13 +6102,13 @@
     </row>
     <row r="179" spans="1:7">
       <c r="A179" t="s">
+        <v>117</v>
+      </c>
+      <c r="B179" t="s">
         <v>118</v>
       </c>
-      <c r="B179" t="s">
-        <v>119</v>
-      </c>
       <c r="C179" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D179" t="s">
         <v>18</v>
@@ -6095,13 +6125,13 @@
     </row>
     <row r="180" spans="1:7">
       <c r="A180" t="s">
+        <v>120</v>
+      </c>
+      <c r="B180" t="s">
         <v>121</v>
       </c>
-      <c r="B180" t="s">
-        <v>122</v>
-      </c>
       <c r="C180" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D180" t="s">
         <v>12</v>
@@ -6118,13 +6148,13 @@
     </row>
     <row r="181" spans="1:7">
       <c r="A181" t="s">
+        <v>120</v>
+      </c>
+      <c r="B181" t="s">
         <v>121</v>
       </c>
-      <c r="B181" t="s">
-        <v>122</v>
-      </c>
       <c r="C181" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D181" t="s">
         <v>12</v>
@@ -6141,13 +6171,13 @@
     </row>
     <row r="182" spans="1:7">
       <c r="A182" t="s">
+        <v>120</v>
+      </c>
+      <c r="B182" t="s">
         <v>121</v>
       </c>
-      <c r="B182" t="s">
-        <v>122</v>
-      </c>
       <c r="C182" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D182" t="s">
         <v>12</v>
@@ -6164,19 +6194,19 @@
     </row>
     <row r="183" spans="1:7">
       <c r="A183" t="s">
+        <v>120</v>
+      </c>
+      <c r="B183" t="s">
         <v>121</v>
       </c>
-      <c r="B183" t="s">
-        <v>122</v>
-      </c>
       <c r="C183" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D183" t="s">
         <v>12</v>
       </c>
       <c r="E183" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F183" t="s">
         <v>136</v>
@@ -6187,13 +6217,13 @@
     </row>
     <row r="184" spans="1:7">
       <c r="A184" t="s">
+        <v>120</v>
+      </c>
+      <c r="B184" t="s">
         <v>121</v>
       </c>
-      <c r="B184" t="s">
-        <v>122</v>
-      </c>
       <c r="C184" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D184" t="s">
         <v>12</v>
@@ -6210,16 +6240,16 @@
     </row>
     <row r="185" spans="1:7">
       <c r="A185" t="s">
+        <v>123</v>
+      </c>
+      <c r="B185" t="s">
         <v>124</v>
       </c>
-      <c r="B185" t="s">
-        <v>125</v>
-      </c>
       <c r="C185" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D185" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E185" t="s">
         <v>131</v>
@@ -6233,16 +6263,16 @@
     </row>
     <row r="186" spans="1:7">
       <c r="A186" t="s">
+        <v>123</v>
+      </c>
+      <c r="B186" t="s">
         <v>124</v>
       </c>
-      <c r="B186" t="s">
-        <v>125</v>
-      </c>
       <c r="C186" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D186" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E186" t="s">
         <v>134</v>
@@ -6256,16 +6286,16 @@
     </row>
     <row r="187" spans="1:7">
       <c r="A187" t="s">
+        <v>123</v>
+      </c>
+      <c r="B187" t="s">
         <v>124</v>
       </c>
-      <c r="B187" t="s">
-        <v>125</v>
-      </c>
       <c r="C187" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D187" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E187" t="s">
         <v>135</v>
@@ -6279,19 +6309,19 @@
     </row>
     <row r="188" spans="1:7">
       <c r="A188" t="s">
+        <v>123</v>
+      </c>
+      <c r="B188" t="s">
         <v>124</v>
       </c>
-      <c r="B188" t="s">
-        <v>125</v>
-      </c>
       <c r="C188" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D188" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E188" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F188" t="s">
         <v>136</v>
@@ -6302,16 +6332,16 @@
     </row>
     <row r="189" spans="1:7">
       <c r="A189" t="s">
+        <v>123</v>
+      </c>
+      <c r="B189" t="s">
         <v>124</v>
       </c>
-      <c r="B189" t="s">
-        <v>125</v>
-      </c>
       <c r="C189" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D189" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E189" t="s">
         <v>139</v>

</xml_diff>